<commit_message>
added to results section
</commit_message>
<xml_diff>
--- a/Final Dataset/FinalDataSet.xlsx
+++ b/Final Dataset/FinalDataSet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/prithvirathaur/Documents/Spring 2020/CS 4641/Project/DataVisualizations/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/prithvirathaur/Documents/Spring 2020/CS 4641/Project/yelpmlproject.github.io/Final Dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DBA0C37-BB60-2C4A-BC41-78276E94ABA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98974C1F-7757-2444-9334-2EEE9F2A11E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -434,7 +434,7 @@
   <dimension ref="A1:M2504"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>